<commit_message>
Updated benchmark results in the report and the xlxs
Former-commit-id: 40b52029e6c794108c8d27d25fa16de0c9d2ac62
</commit_message>
<xml_diff>
--- a/stuffToSendToThem/results_report.xlsx
+++ b/stuffToSendToThem/results_report.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="7740"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="15600" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
   <si>
     <t>Frequency(MHz)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,10 +170,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Group 2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Group 3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -311,13 +307,43 @@
   <si>
     <t>Divisor Upgraded</t>
   </si>
+  <si>
+    <t>Group 1 (mul and div)</t>
+  </si>
+  <si>
+    <t>Wallace</t>
+  </si>
+  <si>
+    <t>2,31s</t>
+  </si>
+  <si>
+    <t>1m52,08s</t>
+  </si>
+  <si>
+    <t>11,50s</t>
+  </si>
+  <si>
+    <t>7,31s</t>
+  </si>
+  <si>
+    <t>5737ms</t>
+  </si>
+  <si>
+    <t>8,60s</t>
+  </si>
+  <si>
+    <t>3m26,92s</t>
+  </si>
+  <si>
+    <t>Divider and Multiplier Upgraded</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -823,6 +849,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -832,23 +861,59 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -868,14 +933,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,58 +948,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Colore 1" xfId="1" builtinId="30"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,7 +973,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1235,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EQ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6:AX8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1275,66 +1301,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:147" s="8" customFormat="1" ht="20.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37"/>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
-      <c r="AV1" s="37"/>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="56" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="50"/>
+      <c r="AQ1" s="50"/>
+      <c r="AR1" s="50"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50"/>
+      <c r="AV1" s="50"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="33" t="s">
         <v>41</v>
       </c>
       <c r="AY1" s="21"/>
@@ -1436,80 +1462,80 @@
       <c r="EQ1" s="21"/>
     </row>
     <row r="2" spans="1:147" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A2" s="54"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="51" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51" t="s">
+      <c r="H2" s="32"/>
+      <c r="I2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51" t="s">
+      <c r="J2" s="32"/>
+      <c r="K2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51" t="s">
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51" t="s">
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM2" s="42"/>
-      <c r="AN2" s="42"/>
-      <c r="AO2" s="42"/>
-      <c r="AP2" s="42"/>
-      <c r="AQ2" s="33"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="56"/>
       <c r="AR2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS2" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="AS2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV2" s="35"/>
-      <c r="AW2" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX2" s="57"/>
+      <c r="AT2" s="56"/>
+      <c r="AU2" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV2" s="62"/>
+      <c r="AW2" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX2" s="34"/>
       <c r="AY2" s="22"/>
       <c r="AZ2" s="22"/>
       <c r="BA2" s="22"/>
@@ -1609,138 +1635,138 @@
       <c r="EQ2" s="22"/>
     </row>
     <row r="3" spans="1:147" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="43" t="s">
+      <c r="S3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="43" t="s">
+      <c r="T3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="43" t="s">
+      <c r="U3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="43" t="s">
+      <c r="V3" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="43" t="s">
+      <c r="W3" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="X3" s="43" t="s">
+      <c r="X3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="Y3" s="43" t="s">
+      <c r="Y3" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="Z3" s="43" t="s">
+      <c r="Z3" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB3" s="43" t="s">
+      <c r="AA3" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="AC3" s="43" t="s">
+      <c r="AC3" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="AD3" s="43" t="s">
+      <c r="AD3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="AE3" s="43" t="s">
+      <c r="AE3" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AF3" s="43" t="s">
+      <c r="AF3" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AG3" s="43" t="s">
+      <c r="AG3" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AH3" s="43" t="s">
+      <c r="AH3" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="AI3" s="43" t="s">
+      <c r="AI3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AJ3" s="43" t="s">
+      <c r="AJ3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AK3" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL3" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM3" s="46"/>
-      <c r="AN3" s="45" t="s">
+      <c r="AK3" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL3" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="AO3" s="46"/>
-      <c r="AP3" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ3" s="33"/>
-      <c r="AR3" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS3" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT3" s="33"/>
-      <c r="AU3" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="AV3" s="35"/>
-      <c r="AW3" s="40"/>
-      <c r="AX3" s="57"/>
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS3" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV3" s="62"/>
+      <c r="AW3" s="53"/>
+      <c r="AX3" s="34"/>
       <c r="AY3" s="22"/>
       <c r="AZ3" s="22"/>
       <c r="BA3" s="22"/>
@@ -1840,76 +1866,76 @@
       <c r="EQ3" s="22"/>
     </row>
     <row r="4" spans="1:147" s="1" customFormat="1" ht="48" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="31"/>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="44"/>
-      <c r="AG4" s="44"/>
-      <c r="AH4" s="44"/>
-      <c r="AI4" s="44"/>
-      <c r="AJ4" s="44"/>
-      <c r="AK4" s="31"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="47"/>
       <c r="AL4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AM4" s="18" t="s">
+      <c r="AN4" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AN4" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="AO4" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AP4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AQ4" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR4" s="31"/>
+      <c r="AR4" s="47"/>
       <c r="AS4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="AT4" s="20" t="s">
-        <v>62</v>
-      </c>
       <c r="AU4" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AV4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="AW4" s="41"/>
-      <c r="AX4" s="58"/>
+        <v>54</v>
+      </c>
+      <c r="AW4" s="54"/>
+      <c r="AX4" s="35"/>
       <c r="AY4" s="23"/>
       <c r="AZ4" s="23"/>
       <c r="BA4" s="23"/>
@@ -2010,10 +2036,10 @@
     </row>
     <row r="5" spans="1:147" s="2" customFormat="1" ht="49.5">
       <c r="A5" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="9">
         <v>5</v>
@@ -2023,7 +2049,7 @@
         <v>35</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="9">
         <v>80.522000000000006</v>
@@ -2046,7 +2072,7 @@
       <c r="M5" s="10">
         <v>3.1880000000000002</v>
       </c>
-      <c r="N5" s="59">
+      <c r="N5" s="27">
         <f>M5/G5</f>
         <v>3.9591664389856188E-2</v>
       </c>
@@ -2087,7 +2113,7 @@
         <v>1021</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB5" s="10">
         <v>0.442</v>
@@ -2117,13 +2143,13 @@
         <v>2.31</v>
       </c>
       <c r="AK5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AL5" s="9">
         <v>781</v>
       </c>
       <c r="AM5" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AN5" s="9">
         <v>15876</v>
@@ -2135,10 +2161,10 @@
         <v>5123</v>
       </c>
       <c r="AQ5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR5" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="AR5" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="AS5" s="9">
         <v>25.28</v>
@@ -2147,16 +2173,16 @@
         <v>21.15</v>
       </c>
       <c r="AU5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="AV5" s="9" t="s">
+      <c r="AW5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="AW5" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="AX5" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AY5" s="24"/>
       <c r="AZ5" s="24"/>
@@ -2257,113 +2283,113 @@
       <c r="EQ5" s="24"/>
     </row>
     <row r="6" spans="1:147" s="3" customFormat="1">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="31" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="49">
+        <v>69</v>
+      </c>
+      <c r="C6" s="31">
         <v>5</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31">
         <v>19</v>
       </c>
-      <c r="F6" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="49">
+      <c r="F6" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="31">
         <v>80.534999999999997</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="31">
         <v>80</v>
       </c>
-      <c r="I6" s="49">
+      <c r="I6" s="31">
         <v>10479</v>
       </c>
-      <c r="J6" s="49">
+      <c r="J6" s="31">
         <v>17865</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="31">
         <v>2.468</v>
       </c>
-      <c r="L6" s="49">
+      <c r="L6" s="31">
         <v>0.74299999999999999</v>
       </c>
-      <c r="M6" s="49">
+      <c r="M6" s="31">
         <v>3.2109999999999999</v>
       </c>
-      <c r="N6" s="60">
+      <c r="N6" s="36">
         <f>M6/G6</f>
         <v>3.9870863599677162E-2</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="28">
         <v>100</v>
       </c>
-      <c r="P6" s="27">
+      <c r="P6" s="28">
         <v>117</v>
       </c>
-      <c r="Q6" s="27">
+      <c r="Q6" s="28">
         <v>83</v>
       </c>
-      <c r="R6" s="27">
+      <c r="R6" s="28">
         <v>84</v>
       </c>
-      <c r="S6" s="27">
+      <c r="S6" s="28">
         <v>800</v>
       </c>
-      <c r="T6" s="27">
+      <c r="T6" s="28">
         <v>717</v>
       </c>
-      <c r="U6" s="27">
+      <c r="U6" s="28">
         <v>83</v>
       </c>
-      <c r="V6" s="27">
+      <c r="V6" s="28">
         <v>150</v>
       </c>
-      <c r="W6" s="27">
+      <c r="W6" s="28">
         <v>434</v>
       </c>
-      <c r="X6" s="27">
+      <c r="X6" s="28">
         <v>1150</v>
       </c>
-      <c r="Y6" s="27">
+      <c r="Y6" s="28">
         <v>257</v>
       </c>
-      <c r="Z6" s="27">
+      <c r="Z6" s="28">
         <v>1002</v>
       </c>
-      <c r="AA6" s="49" t="s">
+      <c r="AA6" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB6" s="28">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="AC6" s="28">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AD6" s="28">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AE6" s="28">
+        <v>0.246</v>
+      </c>
+      <c r="AF6" s="28">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AG6" s="28">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AH6" s="28">
+        <v>1.6579999999999999</v>
+      </c>
+      <c r="AI6" s="28">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="28" t="s">
         <v>80</v>
-      </c>
-      <c r="AB6" s="27">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="AC6" s="27">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="AD6" s="27">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="AE6" s="27">
-        <v>0.246</v>
-      </c>
-      <c r="AF6" s="27">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AG6" s="27">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AH6" s="27">
-        <v>1.6579999999999999</v>
-      </c>
-      <c r="AI6" s="27">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="27" t="s">
-        <v>81</v>
       </c>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15"/>
@@ -2377,8 +2403,8 @@
       <c r="AU6" s="15"/>
       <c r="AV6" s="15"/>
       <c r="AW6" s="15"/>
-      <c r="AX6" s="50" t="s">
-        <v>87</v>
+      <c r="AX6" s="39" t="s">
+        <v>86</v>
       </c>
       <c r="AY6" s="25"/>
       <c r="AZ6" s="25"/>
@@ -2479,92 +2505,92 @@
       <c r="EQ6" s="25"/>
     </row>
     <row r="7" spans="1:147" s="3" customFormat="1">
-      <c r="A7" s="49"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="28">
+        <v>70</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="29">
         <v>100</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="29">
         <v>117</v>
       </c>
-      <c r="Q7" s="28">
+      <c r="Q7" s="29">
         <v>67</v>
       </c>
-      <c r="R7" s="28">
+      <c r="R7" s="29">
         <v>100</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7" s="29">
         <v>816</v>
       </c>
-      <c r="T7" s="28">
+      <c r="T7" s="29">
         <v>717</v>
       </c>
-      <c r="U7" s="28">
+      <c r="U7" s="29">
         <v>83</v>
       </c>
-      <c r="V7" s="28">
+      <c r="V7" s="29">
         <v>150</v>
       </c>
-      <c r="W7" s="28">
+      <c r="W7" s="29">
         <v>434</v>
       </c>
-      <c r="X7" s="28">
+      <c r="X7" s="29">
         <v>1150</v>
       </c>
-      <c r="Y7" s="28">
+      <c r="Y7" s="29">
         <v>257</v>
       </c>
-      <c r="Z7" s="28">
+      <c r="Z7" s="29">
         <v>1006</v>
       </c>
-      <c r="AA7" s="49"/>
-      <c r="AB7" s="28">
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="29">
         <v>0.45400000000000001</v>
       </c>
-      <c r="AC7" s="28">
+      <c r="AC7" s="29">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AD7" s="28">
+      <c r="AD7" s="29">
         <v>0.27400000000000002</v>
       </c>
-      <c r="AE7" s="28">
+      <c r="AE7" s="29">
         <v>0.246</v>
       </c>
-      <c r="AF7" s="28">
+      <c r="AF7" s="29">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AG7" s="28">
+      <c r="AG7" s="29">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AH7" s="28">
+      <c r="AH7" s="29">
         <v>1.68</v>
       </c>
-      <c r="AI7" s="28">
+      <c r="AI7" s="29">
         <v>4.5999999999999996</v>
       </c>
       <c r="AJ7" s="16">
         <v>2.3839999999999999</v>
       </c>
-      <c r="AK7" s="28"/>
+      <c r="AK7" s="29"/>
       <c r="AL7" s="16">
         <v>801</v>
       </c>
       <c r="AM7" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AN7" s="16">
         <v>16335</v>
@@ -2579,7 +2605,7 @@
         <v>10.5</v>
       </c>
       <c r="AR7" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AS7" s="16">
         <v>24.31</v>
@@ -2588,15 +2614,15 @@
         <v>20.62</v>
       </c>
       <c r="AU7" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AV7" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AW7" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="AX7" s="50"/>
+        <v>82</v>
+      </c>
+      <c r="AX7" s="39"/>
       <c r="AY7" s="25"/>
       <c r="AZ7" s="25"/>
       <c r="BA7" s="25"/>
@@ -2696,83 +2722,83 @@
       <c r="EQ7" s="25"/>
     </row>
     <row r="8" spans="1:147" s="3" customFormat="1">
-      <c r="A8" s="49"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="29">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="30">
         <v>100</v>
       </c>
-      <c r="P8" s="29">
+      <c r="P8" s="30">
         <v>117</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="Q8" s="30">
         <v>67</v>
       </c>
-      <c r="R8" s="29">
+      <c r="R8" s="30">
         <v>100</v>
       </c>
-      <c r="S8" s="29">
+      <c r="S8" s="30">
         <v>816</v>
       </c>
-      <c r="T8" s="29">
+      <c r="T8" s="30">
         <v>717</v>
       </c>
-      <c r="U8" s="29">
+      <c r="U8" s="30">
         <v>83</v>
       </c>
-      <c r="V8" s="29">
+      <c r="V8" s="30">
         <v>150</v>
       </c>
-      <c r="W8" s="29">
+      <c r="W8" s="30">
         <v>434</v>
       </c>
-      <c r="X8" s="29">
+      <c r="X8" s="30">
         <v>1150</v>
       </c>
-      <c r="Y8" s="29">
+      <c r="Y8" s="30">
         <v>257</v>
       </c>
-      <c r="Z8" s="29">
+      <c r="Z8" s="30">
         <v>1006</v>
       </c>
-      <c r="AA8" s="49"/>
-      <c r="AB8" s="29">
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="30">
         <v>0.45400000000000001</v>
       </c>
-      <c r="AC8" s="29">
+      <c r="AC8" s="30">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AD8" s="29">
+      <c r="AD8" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="AE8" s="29">
+      <c r="AE8" s="30">
         <v>0.246</v>
       </c>
-      <c r="AF8" s="29">
+      <c r="AF8" s="30">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AG8" s="29">
+      <c r="AG8" s="30">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AH8" s="29">
+      <c r="AH8" s="30">
         <v>1.68</v>
       </c>
-      <c r="AI8" s="29">
+      <c r="AI8" s="30">
         <v>4.5999999999999996</v>
       </c>
       <c r="AJ8" s="17"/>
-      <c r="AK8" s="29"/>
+      <c r="AK8" s="30"/>
       <c r="AL8" s="17"/>
       <c r="AM8" s="17"/>
       <c r="AN8" s="17"/>
@@ -2785,7 +2811,7 @@
       <c r="AU8" s="17"/>
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
-      <c r="AX8" s="50"/>
+      <c r="AX8" s="39"/>
       <c r="AY8" s="25"/>
       <c r="AZ8" s="25"/>
       <c r="BA8" s="25"/>
@@ -2885,58 +2911,145 @@
       <c r="EQ8" s="25"/>
     </row>
     <row r="9" spans="1:147" s="4" customFormat="1">
-      <c r="A9" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="49"/>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="49"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="49"/>
-      <c r="AB9" s="49"/>
-      <c r="AC9" s="49"/>
-      <c r="AD9" s="49"/>
-      <c r="AE9" s="49"/>
-      <c r="AF9" s="49"/>
-      <c r="AG9" s="49"/>
-      <c r="AH9" s="49"/>
-      <c r="AI9" s="49"/>
-      <c r="AJ9" s="27"/>
-      <c r="AK9" s="49"/>
-      <c r="AL9" s="27"/>
-      <c r="AM9" s="27"/>
-      <c r="AN9" s="27"/>
-      <c r="AO9" s="27"/>
-      <c r="AP9" s="27"/>
-      <c r="AQ9" s="27"/>
-      <c r="AR9" s="27"/>
+      <c r="A9" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="31">
+        <v>2</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="31">
+        <v>19</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="31">
+        <v>40.197000000000003</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31">
+        <v>11886</v>
+      </c>
+      <c r="J9" s="31">
+        <v>20469</v>
+      </c>
+      <c r="K9" s="31">
+        <v>2.5110000000000001</v>
+      </c>
+      <c r="L9" s="31">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="M9" s="31">
+        <v>3.343</v>
+      </c>
+      <c r="N9" s="36">
+        <f>M9/G9</f>
+        <v>8.3165410354006514E-2</v>
+      </c>
+      <c r="O9" s="31">
+        <v>100</v>
+      </c>
+      <c r="P9" s="31">
+        <v>117</v>
+      </c>
+      <c r="Q9" s="31">
+        <v>66</v>
+      </c>
+      <c r="R9" s="31">
+        <v>100</v>
+      </c>
+      <c r="S9" s="31">
+        <v>800</v>
+      </c>
+      <c r="T9" s="31">
+        <v>717</v>
+      </c>
+      <c r="U9" s="31">
+        <v>83</v>
+      </c>
+      <c r="V9" s="31">
+        <v>150</v>
+      </c>
+      <c r="W9" s="31">
+        <v>417</v>
+      </c>
+      <c r="X9" s="31">
+        <v>1150</v>
+      </c>
+      <c r="Y9" s="31">
+        <v>252</v>
+      </c>
+      <c r="Z9" s="28">
+        <v>997</v>
+      </c>
+      <c r="AA9" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB9" s="31">
+        <v>0.46</v>
+      </c>
+      <c r="AC9" s="31">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AD9" s="31">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="AE9" s="31">
+        <v>0.247</v>
+      </c>
+      <c r="AF9" s="31">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AG9" s="31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AH9" s="31">
+        <v>1.726</v>
+      </c>
+      <c r="AI9" s="31">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AJ9" s="28">
+        <v>2.31</v>
+      </c>
+      <c r="AK9" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL9" s="28">
+        <v>914</v>
+      </c>
+      <c r="AM9" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN9" s="28">
+        <v>19205</v>
+      </c>
+      <c r="AO9" s="28">
+        <v>10.78</v>
+      </c>
+      <c r="AP9" s="28">
+        <v>5353</v>
+      </c>
+      <c r="AQ9" s="28">
+        <v>10.6</v>
+      </c>
+      <c r="AR9" s="28" t="s">
+        <v>92</v>
+      </c>
       <c r="AS9" s="15"/>
       <c r="AT9" s="15"/>
       <c r="AU9" s="15"/>
       <c r="AV9" s="15"/>
       <c r="AW9" s="15"/>
-      <c r="AX9" s="50"/>
+      <c r="AX9" s="39" t="s">
+        <v>96</v>
+      </c>
       <c r="AY9" s="25"/>
       <c r="AZ9" s="25"/>
       <c r="BA9" s="25"/>
@@ -3036,56 +3149,68 @@
       <c r="EQ9" s="25"/>
     </row>
     <row r="10" spans="1:147" s="4" customFormat="1">
-      <c r="A10" s="49"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="49"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="49"/>
-      <c r="V10" s="49"/>
-      <c r="W10" s="49"/>
-      <c r="X10" s="49"/>
-      <c r="Y10" s="49"/>
-      <c r="Z10" s="28"/>
-      <c r="AA10" s="49"/>
-      <c r="AB10" s="49"/>
-      <c r="AC10" s="49"/>
-      <c r="AD10" s="49"/>
-      <c r="AE10" s="49"/>
-      <c r="AF10" s="49"/>
-      <c r="AG10" s="49"/>
-      <c r="AH10" s="49"/>
-      <c r="AI10" s="49"/>
-      <c r="AJ10" s="28"/>
-      <c r="AK10" s="49"/>
-      <c r="AL10" s="28"/>
-      <c r="AM10" s="28"/>
-      <c r="AN10" s="28"/>
-      <c r="AO10" s="28"/>
-      <c r="AP10" s="28"/>
-      <c r="AQ10" s="28"/>
-      <c r="AR10" s="28"/>
-      <c r="AS10" s="16"/>
-      <c r="AT10" s="16"/>
-      <c r="AU10" s="16"/>
-      <c r="AV10" s="16"/>
-      <c r="AW10" s="16"/>
-      <c r="AX10" s="50"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+      <c r="AG10" s="31"/>
+      <c r="AH10" s="31"/>
+      <c r="AI10" s="31"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="31"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="29"/>
+      <c r="AN10" s="29"/>
+      <c r="AO10" s="29"/>
+      <c r="AP10" s="29"/>
+      <c r="AQ10" s="29"/>
+      <c r="AR10" s="29"/>
+      <c r="AS10" s="16">
+        <v>23.78</v>
+      </c>
+      <c r="AT10" s="16">
+        <v>19.77</v>
+      </c>
+      <c r="AU10" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX10" s="39"/>
       <c r="AY10" s="25"/>
       <c r="AZ10" s="25"/>
       <c r="BA10" s="25"/>
@@ -3185,56 +3310,56 @@
       <c r="EQ10" s="25"/>
     </row>
     <row r="11" spans="1:147" s="4" customFormat="1">
-      <c r="A11" s="49"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="49"/>
-      <c r="V11" s="49"/>
-      <c r="W11" s="49"/>
-      <c r="X11" s="49"/>
-      <c r="Y11" s="49"/>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="49"/>
-      <c r="AB11" s="49"/>
-      <c r="AC11" s="49"/>
-      <c r="AD11" s="49"/>
-      <c r="AE11" s="49"/>
-      <c r="AF11" s="49"/>
-      <c r="AG11" s="49"/>
-      <c r="AH11" s="49"/>
-      <c r="AI11" s="49"/>
-      <c r="AJ11" s="29"/>
-      <c r="AK11" s="49"/>
-      <c r="AL11" s="29"/>
-      <c r="AM11" s="29"/>
-      <c r="AN11" s="29"/>
-      <c r="AO11" s="29"/>
-      <c r="AP11" s="29"/>
-      <c r="AQ11" s="29"/>
-      <c r="AR11" s="29"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="31"/>
+      <c r="AG11" s="31"/>
+      <c r="AH11" s="31"/>
+      <c r="AI11" s="31"/>
+      <c r="AJ11" s="30"/>
+      <c r="AK11" s="31"/>
+      <c r="AL11" s="30"/>
+      <c r="AM11" s="30"/>
+      <c r="AN11" s="30"/>
+      <c r="AO11" s="30"/>
+      <c r="AP11" s="30"/>
+      <c r="AQ11" s="30"/>
+      <c r="AR11" s="30"/>
       <c r="AS11" s="17"/>
       <c r="AT11" s="17"/>
       <c r="AU11" s="17"/>
       <c r="AV11" s="17"/>
       <c r="AW11" s="17"/>
-      <c r="AX11" s="50"/>
+      <c r="AX11" s="39"/>
       <c r="AY11" s="25"/>
       <c r="AZ11" s="25"/>
       <c r="BA11" s="25"/>
@@ -3334,58 +3459,58 @@
       <c r="EQ11" s="25"/>
     </row>
     <row r="12" spans="1:147" s="3" customFormat="1">
-      <c r="A12" s="49" t="s">
-        <v>44</v>
+      <c r="A12" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="49"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
-      <c r="X12" s="49"/>
-      <c r="Y12" s="49"/>
-      <c r="Z12" s="27"/>
-      <c r="AA12" s="49"/>
-      <c r="AB12" s="49"/>
-      <c r="AC12" s="49"/>
-      <c r="AD12" s="49"/>
-      <c r="AE12" s="49"/>
-      <c r="AF12" s="49"/>
-      <c r="AG12" s="49"/>
-      <c r="AH12" s="49"/>
-      <c r="AI12" s="49"/>
-      <c r="AJ12" s="27"/>
-      <c r="AK12" s="49"/>
-      <c r="AL12" s="27"/>
-      <c r="AM12" s="27"/>
-      <c r="AN12" s="27"/>
-      <c r="AO12" s="27"/>
-      <c r="AP12" s="27"/>
-      <c r="AQ12" s="27"/>
-      <c r="AR12" s="27"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="31"/>
+      <c r="AI12" s="31"/>
+      <c r="AJ12" s="28"/>
+      <c r="AK12" s="31"/>
+      <c r="AL12" s="28"/>
+      <c r="AM12" s="28"/>
+      <c r="AN12" s="28"/>
+      <c r="AO12" s="28"/>
+      <c r="AP12" s="28"/>
+      <c r="AQ12" s="28"/>
+      <c r="AR12" s="28"/>
       <c r="AS12" s="15"/>
       <c r="AT12" s="15"/>
       <c r="AU12" s="15"/>
       <c r="AV12" s="15"/>
       <c r="AW12" s="15"/>
-      <c r="AX12" s="50"/>
+      <c r="AX12" s="39"/>
       <c r="AY12" s="25"/>
       <c r="AZ12" s="25"/>
       <c r="BA12" s="25"/>
@@ -3485,56 +3610,56 @@
       <c r="EQ12" s="25"/>
     </row>
     <row r="13" spans="1:147" s="3" customFormat="1">
-      <c r="A13" s="49"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="49"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="49"/>
-      <c r="U13" s="49"/>
-      <c r="V13" s="49"/>
-      <c r="W13" s="49"/>
-      <c r="X13" s="49"/>
-      <c r="Y13" s="49"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="49"/>
-      <c r="AB13" s="49"/>
-      <c r="AC13" s="49"/>
-      <c r="AD13" s="49"/>
-      <c r="AE13" s="49"/>
-      <c r="AF13" s="49"/>
-      <c r="AG13" s="49"/>
-      <c r="AH13" s="49"/>
-      <c r="AI13" s="49"/>
-      <c r="AJ13" s="28"/>
-      <c r="AK13" s="49"/>
-      <c r="AL13" s="28"/>
-      <c r="AM13" s="28"/>
-      <c r="AN13" s="28"/>
-      <c r="AO13" s="28"/>
-      <c r="AP13" s="28"/>
-      <c r="AQ13" s="28"/>
-      <c r="AR13" s="28"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
+      <c r="AE13" s="31"/>
+      <c r="AF13" s="31"/>
+      <c r="AG13" s="31"/>
+      <c r="AH13" s="31"/>
+      <c r="AI13" s="31"/>
+      <c r="AJ13" s="29"/>
+      <c r="AK13" s="31"/>
+      <c r="AL13" s="29"/>
+      <c r="AM13" s="29"/>
+      <c r="AN13" s="29"/>
+      <c r="AO13" s="29"/>
+      <c r="AP13" s="29"/>
+      <c r="AQ13" s="29"/>
+      <c r="AR13" s="29"/>
       <c r="AS13" s="16"/>
       <c r="AT13" s="16"/>
       <c r="AU13" s="16"/>
       <c r="AV13" s="16"/>
       <c r="AW13" s="16"/>
-      <c r="AX13" s="50"/>
+      <c r="AX13" s="39"/>
       <c r="AY13" s="25"/>
       <c r="AZ13" s="25"/>
       <c r="BA13" s="25"/>
@@ -3634,56 +3759,56 @@
       <c r="EQ13" s="25"/>
     </row>
     <row r="14" spans="1:147" s="3" customFormat="1">
-      <c r="A14" s="49"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="49"/>
-      <c r="U14" s="49"/>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
-      <c r="X14" s="49"/>
-      <c r="Y14" s="49"/>
-      <c r="Z14" s="29"/>
-      <c r="AA14" s="49"/>
-      <c r="AB14" s="49"/>
-      <c r="AC14" s="49"/>
-      <c r="AD14" s="49"/>
-      <c r="AE14" s="49"/>
-      <c r="AF14" s="49"/>
-      <c r="AG14" s="49"/>
-      <c r="AH14" s="49"/>
-      <c r="AI14" s="49"/>
-      <c r="AJ14" s="29"/>
-      <c r="AK14" s="49"/>
-      <c r="AL14" s="29"/>
-      <c r="AM14" s="29"/>
-      <c r="AN14" s="29"/>
-      <c r="AO14" s="29"/>
-      <c r="AP14" s="29"/>
-      <c r="AQ14" s="29"/>
-      <c r="AR14" s="29"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="31"/>
+      <c r="AI14" s="31"/>
+      <c r="AJ14" s="30"/>
+      <c r="AK14" s="31"/>
+      <c r="AL14" s="30"/>
+      <c r="AM14" s="30"/>
+      <c r="AN14" s="30"/>
+      <c r="AO14" s="30"/>
+      <c r="AP14" s="30"/>
+      <c r="AQ14" s="30"/>
+      <c r="AR14" s="30"/>
       <c r="AS14" s="17"/>
       <c r="AT14" s="17"/>
       <c r="AU14" s="17"/>
       <c r="AV14" s="17"/>
       <c r="AW14" s="17"/>
-      <c r="AX14" s="50"/>
+      <c r="AX14" s="39"/>
       <c r="AY14" s="25"/>
       <c r="AZ14" s="25"/>
       <c r="BA14" s="25"/>
@@ -3783,58 +3908,58 @@
       <c r="EQ14" s="25"/>
     </row>
     <row r="15" spans="1:147" s="4" customFormat="1">
-      <c r="A15" s="49" t="s">
-        <v>45</v>
+      <c r="A15" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="49"/>
-      <c r="W15" s="49"/>
-      <c r="X15" s="49"/>
-      <c r="Y15" s="49"/>
-      <c r="Z15" s="27"/>
-      <c r="AA15" s="49"/>
-      <c r="AB15" s="49"/>
-      <c r="AC15" s="49"/>
-      <c r="AD15" s="49"/>
-      <c r="AE15" s="49"/>
-      <c r="AF15" s="49"/>
-      <c r="AG15" s="49"/>
-      <c r="AH15" s="49"/>
-      <c r="AI15" s="49"/>
-      <c r="AJ15" s="27"/>
-      <c r="AK15" s="49"/>
-      <c r="AL15" s="27"/>
-      <c r="AM15" s="27"/>
-      <c r="AN15" s="27"/>
-      <c r="AO15" s="27"/>
-      <c r="AP15" s="27"/>
-      <c r="AQ15" s="27"/>
-      <c r="AR15" s="27"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="31"/>
+      <c r="AB15" s="31"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="31"/>
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="31"/>
+      <c r="AG15" s="31"/>
+      <c r="AH15" s="31"/>
+      <c r="AI15" s="31"/>
+      <c r="AJ15" s="28"/>
+      <c r="AK15" s="31"/>
+      <c r="AL15" s="28"/>
+      <c r="AM15" s="28"/>
+      <c r="AN15" s="28"/>
+      <c r="AO15" s="28"/>
+      <c r="AP15" s="28"/>
+      <c r="AQ15" s="28"/>
+      <c r="AR15" s="28"/>
       <c r="AS15" s="15"/>
       <c r="AT15" s="15"/>
       <c r="AU15" s="15"/>
       <c r="AV15" s="15"/>
       <c r="AW15" s="15"/>
-      <c r="AX15" s="50"/>
+      <c r="AX15" s="39"/>
       <c r="AY15" s="25"/>
       <c r="AZ15" s="25"/>
       <c r="BA15" s="25"/>
@@ -3934,56 +4059,56 @@
       <c r="EQ15" s="25"/>
     </row>
     <row r="16" spans="1:147" s="4" customFormat="1">
-      <c r="A16" s="49"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="49"/>
-      <c r="R16" s="49"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="49"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="49"/>
-      <c r="W16" s="49"/>
-      <c r="X16" s="49"/>
-      <c r="Y16" s="49"/>
-      <c r="Z16" s="28"/>
-      <c r="AA16" s="49"/>
-      <c r="AB16" s="49"/>
-      <c r="AC16" s="49"/>
-      <c r="AD16" s="49"/>
-      <c r="AE16" s="49"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="49"/>
-      <c r="AH16" s="49"/>
-      <c r="AI16" s="49"/>
-      <c r="AJ16" s="28"/>
-      <c r="AK16" s="49"/>
-      <c r="AL16" s="28"/>
-      <c r="AM16" s="28"/>
-      <c r="AN16" s="28"/>
-      <c r="AO16" s="28"/>
-      <c r="AP16" s="28"/>
-      <c r="AQ16" s="28"/>
-      <c r="AR16" s="28"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31"/>
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="31"/>
+      <c r="AG16" s="31"/>
+      <c r="AH16" s="31"/>
+      <c r="AI16" s="31"/>
+      <c r="AJ16" s="29"/>
+      <c r="AK16" s="31"/>
+      <c r="AL16" s="29"/>
+      <c r="AM16" s="29"/>
+      <c r="AN16" s="29"/>
+      <c r="AO16" s="29"/>
+      <c r="AP16" s="29"/>
+      <c r="AQ16" s="29"/>
+      <c r="AR16" s="29"/>
       <c r="AS16" s="16"/>
       <c r="AT16" s="16"/>
       <c r="AU16" s="16"/>
       <c r="AV16" s="16"/>
       <c r="AW16" s="16"/>
-      <c r="AX16" s="50"/>
+      <c r="AX16" s="39"/>
       <c r="AY16" s="25"/>
       <c r="AZ16" s="25"/>
       <c r="BA16" s="25"/>
@@ -4083,56 +4208,56 @@
       <c r="EQ16" s="25"/>
     </row>
     <row r="17" spans="1:147" s="4" customFormat="1">
-      <c r="A17" s="49"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="49"/>
-      <c r="R17" s="49"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="49"/>
-      <c r="U17" s="49"/>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
-      <c r="X17" s="49"/>
-      <c r="Y17" s="49"/>
-      <c r="Z17" s="29"/>
-      <c r="AA17" s="49"/>
-      <c r="AB17" s="49"/>
-      <c r="AC17" s="49"/>
-      <c r="AD17" s="49"/>
-      <c r="AE17" s="49"/>
-      <c r="AF17" s="49"/>
-      <c r="AG17" s="49"/>
-      <c r="AH17" s="49"/>
-      <c r="AI17" s="49"/>
-      <c r="AJ17" s="29"/>
-      <c r="AK17" s="49"/>
-      <c r="AL17" s="29"/>
-      <c r="AM17" s="29"/>
-      <c r="AN17" s="29"/>
-      <c r="AO17" s="29"/>
-      <c r="AP17" s="29"/>
-      <c r="AQ17" s="29"/>
-      <c r="AR17" s="29"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="31"/>
+      <c r="AE17" s="31"/>
+      <c r="AF17" s="31"/>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="31"/>
+      <c r="AI17" s="31"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="31"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30"/>
+      <c r="AO17" s="30"/>
+      <c r="AP17" s="30"/>
+      <c r="AQ17" s="30"/>
+      <c r="AR17" s="30"/>
       <c r="AS17" s="17"/>
       <c r="AT17" s="17"/>
       <c r="AU17" s="17"/>
       <c r="AV17" s="17"/>
       <c r="AW17" s="17"/>
-      <c r="AX17" s="50"/>
+      <c r="AX17" s="39"/>
       <c r="AY17" s="25"/>
       <c r="AZ17" s="25"/>
       <c r="BA17" s="25"/>
@@ -4232,58 +4357,58 @@
       <c r="EQ17" s="25"/>
     </row>
     <row r="18" spans="1:147" s="3" customFormat="1">
-      <c r="A18" s="49" t="s">
-        <v>46</v>
+      <c r="A18" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="49"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
-      <c r="X18" s="49"/>
-      <c r="Y18" s="49"/>
-      <c r="Z18" s="27"/>
-      <c r="AA18" s="49"/>
-      <c r="AB18" s="49"/>
-      <c r="AC18" s="49"/>
-      <c r="AD18" s="49"/>
-      <c r="AE18" s="49"/>
-      <c r="AF18" s="49"/>
-      <c r="AG18" s="49"/>
-      <c r="AH18" s="49"/>
-      <c r="AI18" s="49"/>
-      <c r="AJ18" s="27"/>
-      <c r="AK18" s="49"/>
-      <c r="AL18" s="27"/>
-      <c r="AM18" s="27"/>
-      <c r="AN18" s="27"/>
-      <c r="AO18" s="27"/>
-      <c r="AP18" s="27"/>
-      <c r="AQ18" s="27"/>
-      <c r="AR18" s="27"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="31"/>
+      <c r="AI18" s="31"/>
+      <c r="AJ18" s="28"/>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="28"/>
+      <c r="AM18" s="28"/>
+      <c r="AN18" s="28"/>
+      <c r="AO18" s="28"/>
+      <c r="AP18" s="28"/>
+      <c r="AQ18" s="28"/>
+      <c r="AR18" s="28"/>
       <c r="AS18" s="15"/>
       <c r="AT18" s="15"/>
       <c r="AU18" s="15"/>
       <c r="AV18" s="15"/>
       <c r="AW18" s="15"/>
-      <c r="AX18" s="50"/>
+      <c r="AX18" s="39"/>
       <c r="AY18" s="25"/>
       <c r="AZ18" s="25"/>
       <c r="BA18" s="25"/>
@@ -4383,56 +4508,56 @@
       <c r="EQ18" s="25"/>
     </row>
     <row r="19" spans="1:147" s="3" customFormat="1">
-      <c r="A19" s="49"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="49"/>
-      <c r="U19" s="49"/>
-      <c r="V19" s="49"/>
-      <c r="W19" s="49"/>
-      <c r="X19" s="49"/>
-      <c r="Y19" s="49"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="49"/>
-      <c r="AB19" s="49"/>
-      <c r="AC19" s="49"/>
-      <c r="AD19" s="49"/>
-      <c r="AE19" s="49"/>
-      <c r="AF19" s="49"/>
-      <c r="AG19" s="49"/>
-      <c r="AH19" s="49"/>
-      <c r="AI19" s="49"/>
-      <c r="AJ19" s="28"/>
-      <c r="AK19" s="49"/>
-      <c r="AL19" s="28"/>
-      <c r="AM19" s="28"/>
-      <c r="AN19" s="28"/>
-      <c r="AO19" s="28"/>
-      <c r="AP19" s="28"/>
-      <c r="AQ19" s="28"/>
-      <c r="AR19" s="28"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="31"/>
+      <c r="AE19" s="31"/>
+      <c r="AF19" s="31"/>
+      <c r="AG19" s="31"/>
+      <c r="AH19" s="31"/>
+      <c r="AI19" s="31"/>
+      <c r="AJ19" s="29"/>
+      <c r="AK19" s="31"/>
+      <c r="AL19" s="29"/>
+      <c r="AM19" s="29"/>
+      <c r="AN19" s="29"/>
+      <c r="AO19" s="29"/>
+      <c r="AP19" s="29"/>
+      <c r="AQ19" s="29"/>
+      <c r="AR19" s="29"/>
       <c r="AS19" s="16"/>
       <c r="AT19" s="16"/>
       <c r="AU19" s="16"/>
       <c r="AV19" s="16"/>
       <c r="AW19" s="16"/>
-      <c r="AX19" s="50"/>
+      <c r="AX19" s="39"/>
       <c r="AY19" s="25"/>
       <c r="AZ19" s="25"/>
       <c r="BA19" s="25"/>
@@ -4532,56 +4657,56 @@
       <c r="EQ19" s="25"/>
     </row>
     <row r="20" spans="1:147" s="3" customFormat="1">
-      <c r="A20" s="49"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
-      <c r="U20" s="49"/>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
-      <c r="X20" s="49"/>
-      <c r="Y20" s="49"/>
-      <c r="Z20" s="29"/>
-      <c r="AA20" s="49"/>
-      <c r="AB20" s="49"/>
-      <c r="AC20" s="49"/>
-      <c r="AD20" s="49"/>
-      <c r="AE20" s="49"/>
-      <c r="AF20" s="49"/>
-      <c r="AG20" s="49"/>
-      <c r="AH20" s="49"/>
-      <c r="AI20" s="49"/>
-      <c r="AJ20" s="29"/>
-      <c r="AK20" s="49"/>
-      <c r="AL20" s="29"/>
-      <c r="AM20" s="29"/>
-      <c r="AN20" s="29"/>
-      <c r="AO20" s="29"/>
-      <c r="AP20" s="29"/>
-      <c r="AQ20" s="29"/>
-      <c r="AR20" s="29"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="30"/>
+      <c r="AA20" s="31"/>
+      <c r="AB20" s="31"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="31"/>
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="31"/>
+      <c r="AI20" s="31"/>
+      <c r="AJ20" s="30"/>
+      <c r="AK20" s="31"/>
+      <c r="AL20" s="30"/>
+      <c r="AM20" s="30"/>
+      <c r="AN20" s="30"/>
+      <c r="AO20" s="30"/>
+      <c r="AP20" s="30"/>
+      <c r="AQ20" s="30"/>
+      <c r="AR20" s="30"/>
       <c r="AS20" s="17"/>
       <c r="AT20" s="17"/>
       <c r="AU20" s="17"/>
       <c r="AV20" s="17"/>
       <c r="AW20" s="17"/>
-      <c r="AX20" s="50"/>
+      <c r="AX20" s="39"/>
       <c r="AY20" s="25"/>
       <c r="AZ20" s="25"/>
       <c r="BA20" s="25"/>
@@ -9827,20 +9952,238 @@
     </row>
   </sheetData>
   <mergeCells count="270">
-    <mergeCell ref="AI6:AI8"/>
-    <mergeCell ref="Z6:Z8"/>
-    <mergeCell ref="AE6:AE8"/>
-    <mergeCell ref="AF6:AF8"/>
-    <mergeCell ref="AG6:AG8"/>
-    <mergeCell ref="AH6:AH8"/>
-    <mergeCell ref="S6:S8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="U6:U8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="X6:X8"/>
-    <mergeCell ref="Y6:Y8"/>
-    <mergeCell ref="AA6:AA8"/>
+    <mergeCell ref="AR9:AR11"/>
+    <mergeCell ref="AR12:AR14"/>
+    <mergeCell ref="AR15:AR17"/>
+    <mergeCell ref="AR18:AR20"/>
+    <mergeCell ref="AR3:AR4"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="O1:AW1"/>
+    <mergeCell ref="AW2:AW4"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AL2:AQ2"/>
+    <mergeCell ref="AO9:AO11"/>
+    <mergeCell ref="AO12:AO14"/>
+    <mergeCell ref="AO15:AO17"/>
+    <mergeCell ref="AO18:AO20"/>
+    <mergeCell ref="AP9:AP11"/>
+    <mergeCell ref="AP12:AP14"/>
+    <mergeCell ref="AP15:AP17"/>
+    <mergeCell ref="AP18:AP20"/>
+    <mergeCell ref="AQ9:AQ11"/>
+    <mergeCell ref="AQ12:AQ14"/>
+    <mergeCell ref="AQ15:AQ17"/>
+    <mergeCell ref="AQ18:AQ20"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AN12:AN14"/>
+    <mergeCell ref="AN15:AN17"/>
+    <mergeCell ref="AN18:AN20"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AN9:AN11"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="AJ9:AJ11"/>
+    <mergeCell ref="AJ12:AJ14"/>
+    <mergeCell ref="AJ15:AJ17"/>
+    <mergeCell ref="AJ18:AJ20"/>
+    <mergeCell ref="AL9:AL11"/>
+    <mergeCell ref="AL12:AL14"/>
+    <mergeCell ref="AL15:AL17"/>
+    <mergeCell ref="AL18:AL20"/>
+    <mergeCell ref="AM9:AM11"/>
+    <mergeCell ref="AM12:AM14"/>
+    <mergeCell ref="AM15:AM17"/>
+    <mergeCell ref="AM18:AM20"/>
+    <mergeCell ref="AK9:AK11"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="O18:O20"/>
+    <mergeCell ref="P18:P20"/>
+    <mergeCell ref="AX18:AX20"/>
+    <mergeCell ref="AB18:AB20"/>
+    <mergeCell ref="AC18:AC20"/>
+    <mergeCell ref="AD18:AD20"/>
+    <mergeCell ref="AE18:AE20"/>
+    <mergeCell ref="AF18:AF20"/>
+    <mergeCell ref="V18:V20"/>
+    <mergeCell ref="W18:W20"/>
+    <mergeCell ref="X18:X20"/>
+    <mergeCell ref="Y18:Y20"/>
+    <mergeCell ref="AA18:AA20"/>
+    <mergeCell ref="Z18:Z20"/>
+    <mergeCell ref="AG18:AG20"/>
+    <mergeCell ref="AH18:AH20"/>
+    <mergeCell ref="AI18:AI20"/>
+    <mergeCell ref="AK18:AK20"/>
+    <mergeCell ref="Q18:Q20"/>
+    <mergeCell ref="R18:R20"/>
+    <mergeCell ref="S18:S20"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="AH15:AH17"/>
+    <mergeCell ref="AI15:AI17"/>
+    <mergeCell ref="AK15:AK17"/>
+    <mergeCell ref="AX15:AX17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="AC15:AC17"/>
+    <mergeCell ref="AD15:AD17"/>
+    <mergeCell ref="AE15:AE17"/>
+    <mergeCell ref="AF15:AF17"/>
+    <mergeCell ref="AG15:AG17"/>
+    <mergeCell ref="W15:W17"/>
+    <mergeCell ref="X15:X17"/>
+    <mergeCell ref="Y15:Y17"/>
+    <mergeCell ref="AA15:AA17"/>
+    <mergeCell ref="AB15:AB17"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="U15:U17"/>
+    <mergeCell ref="V15:V17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="P15:P17"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="Z15:Z17"/>
+    <mergeCell ref="AI12:AI14"/>
+    <mergeCell ref="AK12:AK14"/>
+    <mergeCell ref="AX12:AX14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="AD12:AD14"/>
+    <mergeCell ref="AE12:AE14"/>
+    <mergeCell ref="AF12:AF14"/>
+    <mergeCell ref="AG12:AG14"/>
+    <mergeCell ref="AH12:AH14"/>
+    <mergeCell ref="X12:X14"/>
+    <mergeCell ref="Y12:Y14"/>
+    <mergeCell ref="AA12:AA14"/>
+    <mergeCell ref="AB12:AB14"/>
+    <mergeCell ref="AC12:AC14"/>
+    <mergeCell ref="S12:S14"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="V12:V14"/>
+    <mergeCell ref="W12:W14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="Z12:Z14"/>
+    <mergeCell ref="AX9:AX11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="AE9:AE11"/>
+    <mergeCell ref="AF9:AF11"/>
+    <mergeCell ref="AG9:AG11"/>
+    <mergeCell ref="AH9:AH11"/>
+    <mergeCell ref="AI9:AI11"/>
+    <mergeCell ref="Y9:Y11"/>
+    <mergeCell ref="AA9:AA11"/>
+    <mergeCell ref="AB9:AB11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="AC9:AC11"/>
+    <mergeCell ref="AD9:AD11"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="W9:W11"/>
+    <mergeCell ref="X9:X11"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="Q9:Q11"/>
+    <mergeCell ref="R9:R11"/>
+    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="Z9:Z11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
     <mergeCell ref="O2:AA2"/>
     <mergeCell ref="AB2:AK2"/>
     <mergeCell ref="AX1:AX4"/>
@@ -9865,238 +10208,20 @@
     <mergeCell ref="AX6:AX8"/>
     <mergeCell ref="AC6:AC8"/>
     <mergeCell ref="AD6:AD8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="AC9:AC11"/>
-    <mergeCell ref="AD9:AD11"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="U9:U11"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="W9:W11"/>
-    <mergeCell ref="X9:X11"/>
-    <mergeCell ref="O9:O11"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="R9:R11"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="Z9:Z11"/>
-    <mergeCell ref="AX9:AX11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="AE9:AE11"/>
-    <mergeCell ref="AF9:AF11"/>
-    <mergeCell ref="AG9:AG11"/>
-    <mergeCell ref="AH9:AH11"/>
-    <mergeCell ref="AI9:AI11"/>
-    <mergeCell ref="Y9:Y11"/>
-    <mergeCell ref="AA9:AA11"/>
-    <mergeCell ref="AB9:AB11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="AB12:AB14"/>
-    <mergeCell ref="AC12:AC14"/>
-    <mergeCell ref="S12:S14"/>
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="V12:V14"/>
-    <mergeCell ref="W12:W14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="Q12:Q14"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="Z12:Z14"/>
-    <mergeCell ref="AI12:AI14"/>
-    <mergeCell ref="AK12:AK14"/>
-    <mergeCell ref="AX12:AX14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="AD12:AD14"/>
-    <mergeCell ref="AE12:AE14"/>
-    <mergeCell ref="AF12:AF14"/>
-    <mergeCell ref="AG12:AG14"/>
-    <mergeCell ref="AH12:AH14"/>
-    <mergeCell ref="X12:X14"/>
-    <mergeCell ref="Y12:Y14"/>
-    <mergeCell ref="AA12:AA14"/>
-    <mergeCell ref="AA15:AA17"/>
-    <mergeCell ref="AB15:AB17"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="U15:U17"/>
-    <mergeCell ref="V15:V17"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="P15:P17"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Z15:Z17"/>
-    <mergeCell ref="AH15:AH17"/>
-    <mergeCell ref="AI15:AI17"/>
-    <mergeCell ref="AK15:AK17"/>
-    <mergeCell ref="AX15:AX17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="AC15:AC17"/>
-    <mergeCell ref="AD15:AD17"/>
-    <mergeCell ref="AE15:AE17"/>
-    <mergeCell ref="AF15:AF17"/>
-    <mergeCell ref="AG15:AG17"/>
-    <mergeCell ref="W15:W17"/>
-    <mergeCell ref="X15:X17"/>
-    <mergeCell ref="Y15:Y17"/>
-    <mergeCell ref="N18:N20"/>
-    <mergeCell ref="O18:O20"/>
-    <mergeCell ref="P18:P20"/>
-    <mergeCell ref="AX18:AX20"/>
-    <mergeCell ref="AB18:AB20"/>
-    <mergeCell ref="AC18:AC20"/>
-    <mergeCell ref="AD18:AD20"/>
-    <mergeCell ref="AE18:AE20"/>
-    <mergeCell ref="AF18:AF20"/>
-    <mergeCell ref="V18:V20"/>
-    <mergeCell ref="W18:W20"/>
-    <mergeCell ref="X18:X20"/>
-    <mergeCell ref="Y18:Y20"/>
-    <mergeCell ref="AA18:AA20"/>
-    <mergeCell ref="Z18:Z20"/>
-    <mergeCell ref="AG18:AG20"/>
-    <mergeCell ref="AH18:AH20"/>
-    <mergeCell ref="AI18:AI20"/>
-    <mergeCell ref="AK18:AK20"/>
-    <mergeCell ref="Q18:Q20"/>
-    <mergeCell ref="R18:R20"/>
-    <mergeCell ref="S18:S20"/>
-    <mergeCell ref="T18:T20"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="AJ9:AJ11"/>
-    <mergeCell ref="AJ12:AJ14"/>
-    <mergeCell ref="AJ15:AJ17"/>
-    <mergeCell ref="AJ18:AJ20"/>
-    <mergeCell ref="AL9:AL11"/>
-    <mergeCell ref="AL12:AL14"/>
-    <mergeCell ref="AL15:AL17"/>
-    <mergeCell ref="AL18:AL20"/>
-    <mergeCell ref="AM9:AM11"/>
-    <mergeCell ref="AM12:AM14"/>
-    <mergeCell ref="AM15:AM17"/>
-    <mergeCell ref="AM18:AM20"/>
-    <mergeCell ref="AK9:AK11"/>
-    <mergeCell ref="AN9:AN11"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="O1:AW1"/>
-    <mergeCell ref="AW2:AW4"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AL2:AQ2"/>
-    <mergeCell ref="AO9:AO11"/>
-    <mergeCell ref="AO12:AO14"/>
-    <mergeCell ref="AO15:AO17"/>
-    <mergeCell ref="AO18:AO20"/>
-    <mergeCell ref="AP9:AP11"/>
-    <mergeCell ref="AP12:AP14"/>
-    <mergeCell ref="AP15:AP17"/>
-    <mergeCell ref="AP18:AP20"/>
-    <mergeCell ref="AQ9:AQ11"/>
-    <mergeCell ref="AQ12:AQ14"/>
-    <mergeCell ref="AQ15:AQ17"/>
-    <mergeCell ref="AQ18:AQ20"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AN12:AN14"/>
-    <mergeCell ref="AN15:AN17"/>
-    <mergeCell ref="AN18:AN20"/>
-    <mergeCell ref="AR9:AR11"/>
-    <mergeCell ref="AR12:AR14"/>
-    <mergeCell ref="AR15:AR17"/>
-    <mergeCell ref="AR18:AR20"/>
-    <mergeCell ref="AR3:AR4"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AI6:AI8"/>
+    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="AF6:AF8"/>
+    <mergeCell ref="AG6:AG8"/>
+    <mergeCell ref="AH6:AH8"/>
+    <mergeCell ref="S6:S8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="X6:X8"/>
+    <mergeCell ref="Y6:Y8"/>
+    <mergeCell ref="AA6:AA8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>